<commit_message>
added comments section, improved design
</commit_message>
<xml_diff>
--- a/to do.xlsx
+++ b/to do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/af24ddc27edd414a/Documents - one drive/PW/5 SEM/WWW PROJEKT/projekt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{0F689C12-783E-4DCE-B6E5-5391889F9F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B0976CE-1035-40B9-B5FE-90A216DDE669}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="8_{0F689C12-783E-4DCE-B6E5-5391889F9F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8837B34E-EA1B-4288-8917-21C42B7FAAD3}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{D276EB43-0143-4330-9574-F82E5BA05CCE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D276EB43-0143-4330-9574-F82E5BA05CCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -296,8 +296,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="d&quot;.&quot;mm&quot;.&quot;yyyy"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00&quot; &quot;[$zł-415];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$zł-415]"/>
+    <numFmt numFmtId="164" formatCode="d&quot;.&quot;mm&quot;.&quot;yyyy"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00&quot; &quot;[$zł-415];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$zł-415]"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -435,7 +435,7 @@
       <name val="Liberation Sans"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -554,6 +554,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor rgb="FFF7D1D5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor rgb="FFFFDBB6"/>
       </patternFill>
     </fill>
   </fills>
@@ -683,7 +689,7 @@
     <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="16" borderId="8" applyNumberFormat="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="18" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
@@ -704,11 +710,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -749,9 +752,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -816,9 +816,6 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -897,12 +894,48 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -915,61 +948,34 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1008,6 +1014,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1352,8 +1362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A09B6D4-70C7-46AF-9FDE-F592B2E42B32}">
   <dimension ref="B1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.6640625" defaultRowHeight="13.8"/>
@@ -1408,613 +1418,619 @@
       </c>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="94">
+      <c r="C3" s="96">
         <v>0.1</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="88">
+      <c r="G3" s="97">
         <v>1</v>
       </c>
-      <c r="H3" s="88">
+      <c r="H3" s="97">
         <v>0.1</v>
       </c>
-      <c r="I3" s="89">
+      <c r="I3" s="98">
         <v>10</v>
       </c>
-      <c r="J3" s="90" t="s">
+      <c r="J3" s="99" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" s="93"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="10" t="s">
+      <c r="B4" s="95"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="95" t="s">
+      <c r="E4" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="90"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="99"/>
     </row>
     <row r="5" spans="2:10">
-      <c r="B5" s="93"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="10" t="s">
+      <c r="B5" s="95"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="90"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="97"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="99"/>
     </row>
     <row r="6" spans="2:10" ht="27.6">
-      <c r="B6" s="93"/>
-      <c r="C6" s="94"/>
-      <c r="D6" s="11" t="s">
+      <c r="B6" s="95"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="95" t="s">
+      <c r="E6" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="89"/>
-      <c r="J6" s="90"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="97"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="99"/>
     </row>
     <row r="7" spans="2:10" ht="69">
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="92">
+      <c r="C7" s="90">
         <v>0.15</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="96" t="s">
+      <c r="E7" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="13">
         <v>0.6</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="13">
         <v>0.09</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="14">
         <v>9</v>
       </c>
-      <c r="J7" s="16"/>
+      <c r="J7" s="15"/>
     </row>
     <row r="8" spans="2:10" ht="27.6">
-      <c r="B8" s="91"/>
-      <c r="C8" s="92"/>
-      <c r="D8" s="17" t="s">
+      <c r="B8" s="89"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="97" t="s">
+      <c r="E8" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19">
+      <c r="F8" s="17"/>
+      <c r="G8" s="18">
         <v>0.2</v>
       </c>
-      <c r="H8" s="19">
-        <v>0</v>
-      </c>
-      <c r="I8" s="20">
-        <v>0</v>
-      </c>
-      <c r="J8" s="21"/>
+      <c r="H8" s="18">
+        <v>0</v>
+      </c>
+      <c r="I8" s="19">
+        <v>0</v>
+      </c>
+      <c r="J8" s="20"/>
     </row>
     <row r="9" spans="2:10" ht="41.4">
-      <c r="B9" s="91"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="22" t="s">
+      <c r="B9" s="89"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="25">
+      <c r="F9" s="22"/>
+      <c r="G9" s="23">
         <v>0.2</v>
       </c>
-      <c r="H9" s="25">
-        <v>0</v>
-      </c>
-      <c r="I9" s="26">
-        <v>0</v>
-      </c>
-      <c r="J9" s="27"/>
+      <c r="H9" s="23">
+        <v>0</v>
+      </c>
+      <c r="I9" s="24">
+        <v>0</v>
+      </c>
+      <c r="J9" s="25"/>
     </row>
     <row r="10" spans="2:10" ht="27.6">
-      <c r="B10" s="82" t="s">
+      <c r="B10" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="83">
+      <c r="C10" s="92">
         <v>0.25</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="26" t="s">
         <v>65</v>
       </c>
       <c r="E10" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="29"/>
-      <c r="G10" s="30">
+      <c r="F10" s="27"/>
+      <c r="G10" s="28">
         <v>0.3</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="28">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="28">
         <v>7.5</v>
       </c>
-      <c r="J10" s="31"/>
+      <c r="J10" s="29"/>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="82"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="28" t="s">
+      <c r="B11" s="91"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="98" t="s">
+      <c r="E11" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="30">
+      <c r="F11" s="27"/>
+      <c r="G11" s="28">
         <v>0.4</v>
       </c>
-      <c r="H11" s="30">
-        <v>0</v>
-      </c>
-      <c r="I11" s="30">
-        <v>0</v>
-      </c>
-      <c r="J11" s="31"/>
+      <c r="H11" s="28">
+        <v>0</v>
+      </c>
+      <c r="I11" s="28">
+        <v>0</v>
+      </c>
+      <c r="J11" s="29"/>
     </row>
     <row r="12" spans="2:10" ht="27.6">
-      <c r="B12" s="82"/>
-      <c r="C12" s="83"/>
-      <c r="D12" s="28" t="s">
+      <c r="B12" s="91"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="98" t="s">
+      <c r="E12" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="29"/>
-      <c r="G12" s="30">
+      <c r="F12" s="27"/>
+      <c r="G12" s="28">
         <v>0.05</v>
       </c>
-      <c r="H12" s="30">
-        <v>0</v>
-      </c>
-      <c r="I12" s="30">
-        <v>0</v>
-      </c>
-      <c r="J12" s="31"/>
+      <c r="H12" s="28">
+        <v>0</v>
+      </c>
+      <c r="I12" s="28">
+        <v>0</v>
+      </c>
+      <c r="J12" s="29"/>
     </row>
     <row r="13" spans="2:10" ht="41.4">
-      <c r="B13" s="82"/>
-      <c r="C13" s="83"/>
-      <c r="D13" s="28" t="s">
+      <c r="B13" s="91"/>
+      <c r="C13" s="92"/>
+      <c r="D13" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="103" t="s">
+      <c r="E13" s="101" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="30">
+      <c r="F13" s="27"/>
+      <c r="G13" s="28">
         <v>0.25</v>
       </c>
-      <c r="H13" s="30">
-        <v>0</v>
-      </c>
-      <c r="I13" s="30">
-        <v>0</v>
-      </c>
-      <c r="J13" s="31"/>
+      <c r="H13" s="28">
+        <v>0</v>
+      </c>
+      <c r="I13" s="28">
+        <v>0</v>
+      </c>
+      <c r="J13" s="29"/>
     </row>
     <row r="14" spans="2:10" ht="27.6">
-      <c r="B14" s="84" t="s">
+      <c r="B14" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="85">
+      <c r="C14" s="94">
         <v>0.3</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="99" t="s">
+      <c r="E14" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="34">
+      <c r="F14" s="31"/>
+      <c r="G14" s="32">
         <v>0.1</v>
       </c>
-      <c r="H14" s="34">
+      <c r="H14" s="32">
         <v>0.03</v>
       </c>
-      <c r="I14" s="34">
+      <c r="I14" s="32">
         <v>3</v>
       </c>
-      <c r="J14" s="35"/>
+      <c r="J14" s="33"/>
     </row>
     <row r="15" spans="2:10">
-      <c r="B15" s="84"/>
-      <c r="C15" s="85"/>
-      <c r="D15" s="36" t="s">
+      <c r="B15" s="93"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="100" t="s">
+      <c r="E15" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="38"/>
-      <c r="G15" s="39">
+      <c r="F15" s="36"/>
+      <c r="G15" s="37">
         <v>0.1</v>
       </c>
-      <c r="H15" s="39">
-        <v>0</v>
-      </c>
-      <c r="I15" s="39">
-        <v>0</v>
-      </c>
-      <c r="J15" s="40"/>
+      <c r="H15" s="37">
+        <v>0</v>
+      </c>
+      <c r="I15" s="37">
+        <v>0</v>
+      </c>
+      <c r="J15" s="38"/>
     </row>
     <row r="16" spans="2:10" ht="27.6">
-      <c r="B16" s="84"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="36" t="s">
+      <c r="B16" s="93"/>
+      <c r="C16" s="94"/>
+      <c r="D16" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="100" t="s">
+      <c r="E16" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="38"/>
-      <c r="G16" s="39">
+      <c r="F16" s="36"/>
+      <c r="G16" s="37">
         <v>0.05</v>
       </c>
-      <c r="H16" s="39">
-        <v>0</v>
-      </c>
-      <c r="I16" s="39">
-        <v>0</v>
-      </c>
-      <c r="J16" s="40"/>
+      <c r="H16" s="37">
+        <v>0</v>
+      </c>
+      <c r="I16" s="37">
+        <v>0</v>
+      </c>
+      <c r="J16" s="38"/>
     </row>
     <row r="17" spans="2:10">
-      <c r="B17" s="84"/>
-      <c r="C17" s="85"/>
-      <c r="D17" s="36" t="s">
+      <c r="B17" s="93"/>
+      <c r="C17" s="94"/>
+      <c r="D17" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="37" t="s">
+      <c r="E17" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="38"/>
-      <c r="G17" s="39">
+      <c r="F17" s="36"/>
+      <c r="G17" s="37">
         <v>0.2</v>
       </c>
-      <c r="H17" s="39">
-        <v>0</v>
-      </c>
-      <c r="I17" s="39">
-        <v>0</v>
-      </c>
-      <c r="J17" s="40"/>
+      <c r="H17" s="37">
+        <v>0</v>
+      </c>
+      <c r="I17" s="37">
+        <v>0</v>
+      </c>
+      <c r="J17" s="38"/>
     </row>
     <row r="18" spans="2:10">
-      <c r="B18" s="84"/>
-      <c r="C18" s="85"/>
-      <c r="D18" s="36" t="s">
+      <c r="B18" s="93"/>
+      <c r="C18" s="94"/>
+      <c r="D18" s="34" t="s">
         <v>73</v>
       </c>
       <c r="E18" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="38"/>
-      <c r="G18" s="39">
+      <c r="F18" s="36"/>
+      <c r="G18" s="37">
         <v>0.15</v>
       </c>
-      <c r="H18" s="39">
-        <v>0</v>
-      </c>
-      <c r="I18" s="39">
-        <v>0</v>
-      </c>
-      <c r="J18" s="40"/>
+      <c r="H18" s="37">
+        <v>0</v>
+      </c>
+      <c r="I18" s="37">
+        <v>0</v>
+      </c>
+      <c r="J18" s="38"/>
     </row>
     <row r="19" spans="2:10">
-      <c r="B19" s="84"/>
-      <c r="C19" s="85"/>
-      <c r="D19" s="36" t="s">
+      <c r="B19" s="93"/>
+      <c r="C19" s="94"/>
+      <c r="D19" s="34" t="s">
         <v>74</v>
       </c>
       <c r="E19" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="38"/>
-      <c r="G19" s="39">
+      <c r="F19" s="36"/>
+      <c r="G19" s="37">
         <v>0.15</v>
       </c>
-      <c r="H19" s="39">
-        <v>0</v>
-      </c>
-      <c r="I19" s="39">
-        <v>0</v>
-      </c>
-      <c r="J19" s="40"/>
+      <c r="H19" s="37">
+        <v>0</v>
+      </c>
+      <c r="I19" s="37">
+        <v>0</v>
+      </c>
+      <c r="J19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="27.6">
-      <c r="B20" s="84"/>
-      <c r="C20" s="85"/>
-      <c r="D20" s="36" t="s">
+      <c r="B20" s="93"/>
+      <c r="C20" s="94"/>
+      <c r="D20" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="E20" s="100" t="s">
+      <c r="E20" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="38" t="s">
+      <c r="F20" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="39">
+      <c r="G20" s="37">
         <v>0.1</v>
       </c>
-      <c r="H20" s="39">
-        <v>0</v>
-      </c>
-      <c r="I20" s="39">
-        <v>0</v>
-      </c>
-      <c r="J20" s="40"/>
+      <c r="H20" s="37">
+        <v>0</v>
+      </c>
+      <c r="I20" s="37">
+        <v>0</v>
+      </c>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="2:10" ht="41.4">
-      <c r="B21" s="84"/>
-      <c r="C21" s="85"/>
-      <c r="D21" s="41" t="s">
+      <c r="B21" s="93"/>
+      <c r="C21" s="94"/>
+      <c r="D21" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="101" t="s">
+      <c r="E21" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="42"/>
-      <c r="G21" s="43">
+      <c r="F21" s="40"/>
+      <c r="G21" s="41">
         <v>0.15</v>
       </c>
-      <c r="H21" s="43">
-        <v>0</v>
-      </c>
-      <c r="I21" s="43">
-        <v>0</v>
-      </c>
-      <c r="J21" s="44"/>
+      <c r="H21" s="41">
+        <v>0</v>
+      </c>
+      <c r="I21" s="41">
+        <v>0</v>
+      </c>
+      <c r="J21" s="42"/>
     </row>
     <row r="22" spans="2:10" ht="55.2">
-      <c r="B22" s="86" t="s">
+      <c r="B22" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="87">
+      <c r="C22" s="86">
         <v>0.2</v>
       </c>
-      <c r="D22" s="45" t="s">
+      <c r="D22" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="102" t="s">
+      <c r="E22" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="46" t="s">
+      <c r="F22" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="47">
+      <c r="G22" s="45">
         <v>0.5</v>
       </c>
-      <c r="H22" s="47">
+      <c r="H22" s="45">
         <v>0.1</v>
       </c>
-      <c r="I22" s="47">
+      <c r="I22" s="45">
         <v>10</v>
       </c>
-      <c r="J22" s="48"/>
+      <c r="J22" s="46"/>
     </row>
     <row r="23" spans="2:10" ht="55.2">
-      <c r="B23" s="86"/>
-      <c r="C23" s="87"/>
-      <c r="D23" s="49" t="s">
+      <c r="B23" s="85"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="50" t="s">
+      <c r="E23" s="100" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="51" t="s">
+      <c r="F23" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="52">
+      <c r="G23" s="49">
         <v>0.3</v>
       </c>
-      <c r="H23" s="52">
-        <v>0</v>
-      </c>
-      <c r="I23" s="52">
-        <v>0</v>
-      </c>
-      <c r="J23" s="53"/>
+      <c r="H23" s="49">
+        <v>0</v>
+      </c>
+      <c r="I23" s="49">
+        <v>0</v>
+      </c>
+      <c r="J23" s="50"/>
     </row>
     <row r="24" spans="2:10">
-      <c r="B24" s="86"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="54" t="s">
+      <c r="B24" s="85"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="E24" s="55" t="s">
+      <c r="E24" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="56"/>
-      <c r="G24" s="57">
+      <c r="F24" s="53"/>
+      <c r="G24" s="54">
         <v>0.2</v>
       </c>
-      <c r="H24" s="57">
-        <v>0</v>
-      </c>
-      <c r="I24" s="57">
-        <v>0</v>
-      </c>
-      <c r="J24" s="58"/>
+      <c r="H24" s="54">
+        <v>0</v>
+      </c>
+      <c r="I24" s="54">
+        <v>0</v>
+      </c>
+      <c r="J24" s="55"/>
     </row>
     <row r="25" spans="2:10" hidden="1">
-      <c r="B25" s="80" t="s">
+      <c r="B25" s="87" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="88">
         <v>0.1</v>
       </c>
-      <c r="D25" s="59" t="s">
+      <c r="D25" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="E25" s="60" t="s">
+      <c r="E25" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="61"/>
-      <c r="G25" s="62">
+      <c r="F25" s="58"/>
+      <c r="G25" s="59">
         <v>0.1</v>
       </c>
-      <c r="H25" s="62" t="s">
+      <c r="H25" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="I25" s="62">
+      <c r="I25" s="59">
         <v>1</v>
       </c>
-      <c r="J25" s="63"/>
+      <c r="J25" s="60"/>
     </row>
     <row r="26" spans="2:10" ht="41.4" hidden="1">
-      <c r="B26" s="80"/>
-      <c r="C26" s="81"/>
-      <c r="D26" s="64" t="s">
+      <c r="B26" s="87"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="65" t="s">
+      <c r="E26" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="F26" s="66"/>
-      <c r="G26" s="67">
+      <c r="F26" s="63"/>
+      <c r="G26" s="64">
         <v>0.2</v>
       </c>
-      <c r="H26" s="67" t="s">
+      <c r="H26" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="I26" s="67">
+      <c r="I26" s="64">
         <v>2</v>
       </c>
-      <c r="J26" s="68"/>
+      <c r="J26" s="65"/>
     </row>
     <row r="27" spans="2:10" ht="27.6" hidden="1">
-      <c r="B27" s="80"/>
-      <c r="C27" s="81"/>
-      <c r="D27" s="64" t="s">
+      <c r="B27" s="87"/>
+      <c r="C27" s="88"/>
+      <c r="D27" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="E27" s="69" t="s">
+      <c r="E27" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="66"/>
-      <c r="G27" s="70">
+      <c r="F27" s="63"/>
+      <c r="G27" s="67">
         <v>0.2</v>
       </c>
-      <c r="H27" s="67" t="s">
+      <c r="H27" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="I27" s="67">
+      <c r="I27" s="64">
         <v>2</v>
       </c>
-      <c r="J27" s="68"/>
+      <c r="J27" s="65"/>
     </row>
     <row r="28" spans="2:10" hidden="1">
-      <c r="B28" s="80"/>
-      <c r="C28" s="81"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="72" t="s">
+      <c r="B28" s="87"/>
+      <c r="C28" s="88"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="F28" s="66"/>
-      <c r="G28" s="70"/>
-      <c r="H28" s="67"/>
-      <c r="I28" s="67"/>
-      <c r="J28" s="68"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="64"/>
+      <c r="I28" s="64"/>
+      <c r="J28" s="65"/>
     </row>
     <row r="29" spans="2:10" hidden="1">
-      <c r="B29" s="80"/>
-      <c r="C29" s="81"/>
-      <c r="D29" s="64"/>
-      <c r="E29" s="72" t="s">
+      <c r="B29" s="87"/>
+      <c r="C29" s="88"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="F29" s="66"/>
-      <c r="G29" s="70"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="67"/>
-      <c r="J29" s="68"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="65"/>
     </row>
     <row r="30" spans="2:10" ht="27.6" hidden="1">
-      <c r="B30" s="80"/>
-      <c r="C30" s="81"/>
-      <c r="D30" s="71" t="s">
+      <c r="B30" s="87"/>
+      <c r="C30" s="88"/>
+      <c r="D30" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="E30" s="72" t="s">
+      <c r="E30" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="F30" s="73" t="s">
+      <c r="F30" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="G30" s="74">
+      <c r="G30" s="71">
         <v>0.5</v>
       </c>
-      <c r="H30" s="75" t="s">
+      <c r="H30" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="I30" s="75">
+      <c r="I30" s="72">
         <v>5</v>
       </c>
-      <c r="J30" s="76"/>
+      <c r="J30" s="73"/>
     </row>
     <row r="31" spans="2:10">
-      <c r="B31" s="77" t="s">
+      <c r="B31" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="78">
+      <c r="C31" s="75">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D31" s="78"/>
-      <c r="I31" s="79">
+      <c r="D31" s="75"/>
+      <c r="I31" s="76">
         <v>49.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="J3:J6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="G3:G6"/>
+    <mergeCell ref="H3:H6"/>
+    <mergeCell ref="I3:I6"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="B25:B30"/>
@@ -2025,12 +2041,6 @@
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="B14:B21"/>
     <mergeCell ref="C14:C21"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="G3:G6"/>
-    <mergeCell ref="H3:H6"/>
-    <mergeCell ref="I3:I6"/>
-    <mergeCell ref="J3:J6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39370078740157505" bottom="0.39370078740157505" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added logo in header
</commit_message>
<xml_diff>
--- a/to do.xlsx
+++ b/to do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/af24ddc27edd414a/Documents - one drive/PW/5 SEM/WWW PROJEKT/projekt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{0F689C12-783E-4DCE-B6E5-5391889F9F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8837B34E-EA1B-4288-8917-21C42B7FAAD3}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{0F689C12-783E-4DCE-B6E5-5391889F9F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD06ECC0-140F-4899-8290-DC90199EA32C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D276EB43-0143-4330-9574-F82E5BA05CCE}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{D276EB43-0143-4330-9574-F82E5BA05CCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,23 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
   <si>
     <t>projekt do zrobienia</t>
   </si>
   <si>
-    <t>dodac plikc css ze stylami napisanymi samodzielnie nie przez bootstrap</t>
-  </si>
-  <si>
-    <t>dodac walidacje uzytkownikow plus weryfikacja maila</t>
-  </si>
-  <si>
-    <t>dodac mozliwosc komentarzy????</t>
-  </si>
-  <si>
-    <t>dodac mozliwosc uploadowania zdjec do posta</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -289,6 +277,9 @@
   </si>
   <si>
     <t>7-4</t>
+  </si>
+  <si>
+    <t>logo się minimalnie przesuwa jak zmieniam strone</t>
   </si>
 </sst>
 </file>
@@ -918,6 +909,21 @@
     <xf numFmtId="0" fontId="5" fillId="20" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -948,6 +954,9 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -959,24 +968,6 @@
     </xf>
     <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="22">
@@ -1317,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C117BC4D-E61C-4D4C-A7A1-2309B61148B5}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A2:A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1335,22 +1326,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1362,8 +1338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A09B6D4-70C7-46AF-9FDE-F592B2E42B32}">
   <dimension ref="B1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.6640625" defaultRowHeight="13.8"/>
@@ -1390,124 +1366,124 @@
     </row>
     <row r="2" spans="2:10" ht="41.4">
       <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="5" t="s">
+    </row>
+    <row r="3" spans="2:10">
+      <c r="B3" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="C3" s="102">
+        <v>0.1</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="F3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="G3" s="103">
+        <v>1</v>
+      </c>
+      <c r="H3" s="103">
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="104">
+        <v>10</v>
+      </c>
+      <c r="J3" s="100" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:10">
-      <c r="B3" s="95" t="s">
+    <row r="4" spans="2:10">
+      <c r="B4" s="101"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="96">
-        <v>0.1</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="F4" s="8"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="100"/>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" s="101"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="77" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="103"/>
+      <c r="I5" s="104"/>
+      <c r="J5" s="100"/>
+    </row>
+    <row r="6" spans="2:10" ht="27.6">
+      <c r="B6" s="101"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="103"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="104"/>
+      <c r="J6" s="100"/>
+    </row>
+    <row r="7" spans="2:10" ht="69">
+      <c r="B7" s="94" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="95">
+        <v>0.15</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="77" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="97">
-        <v>1</v>
-      </c>
-      <c r="H3" s="97">
-        <v>0.1</v>
-      </c>
-      <c r="I3" s="98">
-        <v>10</v>
-      </c>
-      <c r="J3" s="99" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10">
-      <c r="B4" s="95"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="77" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="99"/>
-    </row>
-    <row r="5" spans="2:10">
-      <c r="B5" s="95"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="77" t="s">
+      <c r="E7" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="99"/>
-    </row>
-    <row r="6" spans="2:10" ht="27.6">
-      <c r="B6" s="95"/>
-      <c r="C6" s="96"/>
-      <c r="D6" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="77" t="s">
+      <c r="F7" s="12" t="s">
         <v>20</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="97"/>
-      <c r="H6" s="97"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="99"/>
-    </row>
-    <row r="7" spans="2:10" ht="69">
-      <c r="B7" s="89" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="90">
-        <v>0.15</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="78" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>24</v>
       </c>
       <c r="G7" s="13">
         <v>0.6</v>
@@ -1521,13 +1497,13 @@
       <c r="J7" s="15"/>
     </row>
     <row r="8" spans="2:10" ht="27.6">
-      <c r="B8" s="89"/>
-      <c r="C8" s="90"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="95"/>
       <c r="D8" s="16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E8" s="79" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="18">
@@ -1542,13 +1518,13 @@
       <c r="J8" s="20"/>
     </row>
     <row r="9" spans="2:10" ht="41.4">
-      <c r="B9" s="89"/>
-      <c r="C9" s="90"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="95"/>
       <c r="D9" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="102" t="s">
-        <v>26</v>
+        <v>60</v>
+      </c>
+      <c r="E9" s="87" t="s">
+        <v>22</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="23">
@@ -1563,17 +1539,17 @@
       <c r="J9" s="25"/>
     </row>
     <row r="10" spans="2:10" ht="27.6">
-      <c r="B10" s="91" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="92">
+      <c r="B10" s="96" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="97">
         <v>0.25</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="103" t="s">
-        <v>28</v>
+        <v>61</v>
+      </c>
+      <c r="E10" s="88" t="s">
+        <v>24</v>
       </c>
       <c r="F10" s="27"/>
       <c r="G10" s="28">
@@ -1588,13 +1564,13 @@
       <c r="J10" s="29"/>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="91"/>
-      <c r="C11" s="92"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="97"/>
       <c r="D11" s="26" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E11" s="80" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F11" s="27"/>
       <c r="G11" s="28">
@@ -1609,13 +1585,13 @@
       <c r="J11" s="29"/>
     </row>
     <row r="12" spans="2:10" ht="27.6">
-      <c r="B12" s="91"/>
-      <c r="C12" s="92"/>
+      <c r="B12" s="96"/>
+      <c r="C12" s="97"/>
       <c r="D12" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E12" s="80" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F12" s="27"/>
       <c r="G12" s="28">
@@ -1630,13 +1606,13 @@
       <c r="J12" s="29"/>
     </row>
     <row r="13" spans="2:10" ht="41.4">
-      <c r="B13" s="91"/>
-      <c r="C13" s="92"/>
+      <c r="B13" s="96"/>
+      <c r="C13" s="97"/>
       <c r="D13" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="101" t="s">
-        <v>31</v>
+        <v>64</v>
+      </c>
+      <c r="E13" s="86" t="s">
+        <v>27</v>
       </c>
       <c r="F13" s="27"/>
       <c r="G13" s="28">
@@ -1651,17 +1627,17 @@
       <c r="J13" s="29"/>
     </row>
     <row r="14" spans="2:10" ht="27.6">
-      <c r="B14" s="93" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="94">
+      <c r="B14" s="98" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="99">
         <v>0.3</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E14" s="81" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F14" s="31"/>
       <c r="G14" s="32">
@@ -1676,13 +1652,13 @@
       <c r="J14" s="33"/>
     </row>
     <row r="15" spans="2:10">
-      <c r="B15" s="93"/>
-      <c r="C15" s="94"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="99"/>
       <c r="D15" s="34" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E15" s="82" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F15" s="36"/>
       <c r="G15" s="37">
@@ -1697,13 +1673,13 @@
       <c r="J15" s="38"/>
     </row>
     <row r="16" spans="2:10" ht="27.6">
-      <c r="B16" s="93"/>
-      <c r="C16" s="94"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="99"/>
       <c r="D16" s="34" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E16" s="82" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F16" s="36"/>
       <c r="G16" s="37">
@@ -1718,13 +1694,13 @@
       <c r="J16" s="38"/>
     </row>
     <row r="17" spans="2:10">
-      <c r="B17" s="93"/>
-      <c r="C17" s="94"/>
+      <c r="B17" s="98"/>
+      <c r="C17" s="99"/>
       <c r="D17" s="34" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F17" s="36"/>
       <c r="G17" s="37">
@@ -1739,13 +1715,13 @@
       <c r="J17" s="38"/>
     </row>
     <row r="18" spans="2:10">
-      <c r="B18" s="93"/>
-      <c r="C18" s="94"/>
+      <c r="B18" s="98"/>
+      <c r="C18" s="99"/>
       <c r="D18" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" s="104" t="s">
-        <v>37</v>
+        <v>69</v>
+      </c>
+      <c r="E18" s="89" t="s">
+        <v>33</v>
       </c>
       <c r="F18" s="36"/>
       <c r="G18" s="37">
@@ -1760,13 +1736,13 @@
       <c r="J18" s="38"/>
     </row>
     <row r="19" spans="2:10">
-      <c r="B19" s="93"/>
-      <c r="C19" s="94"/>
+      <c r="B19" s="98"/>
+      <c r="C19" s="99"/>
       <c r="D19" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="E19" s="104" t="s">
-        <v>38</v>
+        <v>70</v>
+      </c>
+      <c r="E19" s="89" t="s">
+        <v>34</v>
       </c>
       <c r="F19" s="36"/>
       <c r="G19" s="37">
@@ -1781,16 +1757,16 @@
       <c r="J19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="27.6">
-      <c r="B20" s="93"/>
-      <c r="C20" s="94"/>
+      <c r="B20" s="98"/>
+      <c r="C20" s="99"/>
       <c r="D20" s="34" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E20" s="82" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F20" s="36" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G20" s="37">
         <v>0.1</v>
@@ -1804,13 +1780,13 @@
       <c r="J20" s="38"/>
     </row>
     <row r="21" spans="2:10" ht="41.4">
-      <c r="B21" s="93"/>
-      <c r="C21" s="94"/>
+      <c r="B21" s="98"/>
+      <c r="C21" s="99"/>
       <c r="D21" s="39" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E21" s="83" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F21" s="40"/>
       <c r="G21" s="41">
@@ -1825,20 +1801,20 @@
       <c r="J21" s="42"/>
     </row>
     <row r="22" spans="2:10" ht="55.2">
-      <c r="B22" s="85" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="86">
+      <c r="B22" s="90" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="91">
         <v>0.2</v>
       </c>
       <c r="D22" s="43" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E22" s="84" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F22" s="44" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G22" s="45">
         <v>0.5</v>
@@ -1852,16 +1828,16 @@
       <c r="J22" s="46"/>
     </row>
     <row r="23" spans="2:10" ht="55.2">
-      <c r="B23" s="85"/>
-      <c r="C23" s="86"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="91"/>
       <c r="D23" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="E23" s="100" t="s">
-        <v>45</v>
+        <v>74</v>
+      </c>
+      <c r="E23" s="85" t="s">
+        <v>41</v>
       </c>
       <c r="F23" s="48" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G23" s="49">
         <v>0.3</v>
@@ -1875,13 +1851,13 @@
       <c r="J23" s="50"/>
     </row>
     <row r="24" spans="2:10">
-      <c r="B24" s="85"/>
-      <c r="C24" s="86"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="91"/>
       <c r="D24" s="51" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E24" s="52" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F24" s="53"/>
       <c r="G24" s="54">
@@ -1895,79 +1871,79 @@
       </c>
       <c r="J24" s="55"/>
     </row>
-    <row r="25" spans="2:10" hidden="1">
-      <c r="B25" s="87" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="88">
+    <row r="25" spans="2:10">
+      <c r="B25" s="92" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="93">
         <v>0.1</v>
       </c>
       <c r="D25" s="56" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E25" s="57" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F25" s="58"/>
       <c r="G25" s="59">
         <v>0.1</v>
       </c>
       <c r="H25" s="59" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I25" s="59">
         <v>1</v>
       </c>
       <c r="J25" s="60"/>
     </row>
-    <row r="26" spans="2:10" ht="41.4" hidden="1">
-      <c r="B26" s="87"/>
-      <c r="C26" s="88"/>
+    <row r="26" spans="2:10" ht="41.4">
+      <c r="B26" s="92"/>
+      <c r="C26" s="93"/>
       <c r="D26" s="61" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E26" s="62" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F26" s="63"/>
       <c r="G26" s="64">
         <v>0.2</v>
       </c>
       <c r="H26" s="64" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I26" s="64">
         <v>2</v>
       </c>
       <c r="J26" s="65"/>
     </row>
-    <row r="27" spans="2:10" ht="27.6" hidden="1">
-      <c r="B27" s="87"/>
-      <c r="C27" s="88"/>
+    <row r="27" spans="2:10" ht="27.6">
+      <c r="B27" s="92"/>
+      <c r="C27" s="93"/>
       <c r="D27" s="61" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E27" s="66" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F27" s="63"/>
       <c r="G27" s="67">
         <v>0.2</v>
       </c>
       <c r="H27" s="64" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I27" s="64">
         <v>2</v>
       </c>
       <c r="J27" s="65"/>
     </row>
-    <row r="28" spans="2:10" hidden="1">
-      <c r="B28" s="87"/>
-      <c r="C28" s="88"/>
+    <row r="28" spans="2:10">
+      <c r="B28" s="92"/>
+      <c r="C28" s="93"/>
       <c r="D28" s="61"/>
       <c r="E28" s="69" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F28" s="63"/>
       <c r="G28" s="67"/>
@@ -1975,12 +1951,12 @@
       <c r="I28" s="64"/>
       <c r="J28" s="65"/>
     </row>
-    <row r="29" spans="2:10" hidden="1">
-      <c r="B29" s="87"/>
-      <c r="C29" s="88"/>
+    <row r="29" spans="2:10">
+      <c r="B29" s="92"/>
+      <c r="C29" s="93"/>
       <c r="D29" s="61"/>
       <c r="E29" s="69" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F29" s="63"/>
       <c r="G29" s="67"/>
@@ -1988,23 +1964,23 @@
       <c r="I29" s="64"/>
       <c r="J29" s="65"/>
     </row>
-    <row r="30" spans="2:10" ht="27.6" hidden="1">
-      <c r="B30" s="87"/>
-      <c r="C30" s="88"/>
+    <row r="30" spans="2:10" ht="27.6">
+      <c r="B30" s="92"/>
+      <c r="C30" s="93"/>
       <c r="D30" s="68" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E30" s="69" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F30" s="70" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G30" s="71">
         <v>0.5</v>
       </c>
       <c r="H30" s="72" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I30" s="72">
         <v>5</v>
@@ -2013,7 +1989,7 @@
     </row>
     <row r="31" spans="2:10">
       <c r="B31" s="74" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C31" s="75">
         <v>1.1000000000000001</v>

</xml_diff>